<commit_message>
PBDS-7073 Add Sum(Number...). Sum of bytes and shorts should return integers
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/MathStatistics.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/MathStatistics.xlsx
@@ -1,30 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\MathStatistics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="10995" windowWidth="24915" xWindow="120" yWindow="120"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="10995" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="median" r:id="rId1" sheetId="10"/>
-    <sheet name="avg" r:id="rId2" sheetId="15"/>
-    <sheet name="sum" r:id="rId3" sheetId="13"/>
-    <sheet name="product" r:id="rId4" sheetId="14"/>
-    <sheet name="big" r:id="rId5" sheetId="11"/>
-    <sheet name="small" r:id="rId6" sheetId="12"/>
+    <sheet name="median" sheetId="10" r:id="rId1"/>
+    <sheet name="avg" sheetId="15" r:id="rId2"/>
+    <sheet name="product" sheetId="14" r:id="rId3"/>
+    <sheet name="big" sheetId="11" r:id="rId4"/>
+    <sheet name="small" sheetId="12" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="234">
   <si>
     <t>_res_</t>
   </si>
@@ -422,117 +416,6 @@
     <t>Method BigDecimalValue smallBigDecimalValue(BigDecimalValue[] mydata, int pos)</t>
   </si>
   <si>
-    <t>Method byte sumbyte(byte[] mydata)</t>
-  </si>
-  <si>
-    <t>Test sumbyte</t>
-  </si>
-  <si>
-    <t>Test sumByte</t>
-  </si>
-  <si>
-    <t>Test sumByteValue</t>
-  </si>
-  <si>
-    <t>return sum(mydata);</t>
-  </si>
-  <si>
-    <t>Method Byte sumByte(Byte[] mydata)</t>
-  </si>
-  <si>
-    <t>Method ByteValue sumByteValue(ByteValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method short sumshort(short[] mydata)</t>
-  </si>
-  <si>
-    <t>Test sumshort</t>
-  </si>
-  <si>
-    <t>Test sumShort</t>
-  </si>
-  <si>
-    <t>Test sumShortValue</t>
-  </si>
-  <si>
-    <t>Method Short sumShort(Short[] mydata)</t>
-  </si>
-  <si>
-    <t>Method ShortValue sumShortValue(ShortValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method int sumint(int[] mydata)</t>
-  </si>
-  <si>
-    <t>Test sumint</t>
-  </si>
-  <si>
-    <t>Test sumInteger</t>
-  </si>
-  <si>
-    <t>Test sumIntValue</t>
-  </si>
-  <si>
-    <t>Method Integer sumInteger(Integer[] mydata)</t>
-  </si>
-  <si>
-    <t>Method IntValue sumIntValue(IntValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method long sumlong(long[] mydata)</t>
-  </si>
-  <si>
-    <t>Test sumlong</t>
-  </si>
-  <si>
-    <t>Test sumLong</t>
-  </si>
-  <si>
-    <t>Test sumLongValue</t>
-  </si>
-  <si>
-    <t>Method Long sumLong(Long[] mydata)</t>
-  </si>
-  <si>
-    <t>Method LongValue sumLongValue(LongValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method float sumfloat(float[] mydata)</t>
-  </si>
-  <si>
-    <t>Test sumfloat</t>
-  </si>
-  <si>
-    <t>Test sumFloat</t>
-  </si>
-  <si>
-    <t>Test sumFloatValue</t>
-  </si>
-  <si>
-    <t>Method Float sumFloat(Float[] mydata)</t>
-  </si>
-  <si>
-    <t>Method FloatValue sumFloatValue(FloatValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method double sumdouble(double[] mydata)</t>
-  </si>
-  <si>
-    <t>Test sumdouble</t>
-  </si>
-  <si>
-    <t>Test sumDouble</t>
-  </si>
-  <si>
-    <t>Test sumDoubleValue</t>
-  </si>
-  <si>
-    <t>Method Double sumDouble(Double[] mydata)</t>
-  </si>
-  <si>
-    <t>Method DoubleValue sumDoubleValue(DoubleValue[] mydata)</t>
-  </si>
-  <si>
     <t>Test productbyte</t>
   </si>
   <si>
@@ -642,30 +525,6 @@
   </si>
   <si>
     <t>Method DoubleValue productByteValue(ByteValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Test sumBigIntegerValue</t>
-  </si>
-  <si>
-    <t>Test sumBigInteger</t>
-  </si>
-  <si>
-    <t>Test sumBigDecimal</t>
-  </si>
-  <si>
-    <t>Test sumBigDecimalValue</t>
-  </si>
-  <si>
-    <t>Method BigDecimal sumBigDecimal(BigDecimal[] mydata)</t>
-  </si>
-  <si>
-    <t>Method BigDecimalValue sumBigDecimalValue(BigDecimalValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method BigIntegerValue sumBigIntegerValue(BigIntegerValue[] mydata)</t>
-  </si>
-  <si>
-    <t>Method BigInteger sumBigInteger(BigInteger[] mydata)</t>
   </si>
   <si>
     <t>Method BigInteger productBigInteger(BigInteger[] mydata)</t>
@@ -866,12 +725,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color rgb="000000" theme="1"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -976,48 +834,48 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyBorder="1" borderId="6" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" borderId="2" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="3" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="4" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1030,14 +888,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1070,9 +928,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1105,26 +963,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1157,26 +998,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1229,7 +1053,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -1238,13 +1062,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1254,7 +1078,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1263,7 +1087,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1272,7 +1096,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1282,12 +1106,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -1318,7 +1142,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -1337,7 +1161,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -1349,8 +1173,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K105"/>
   <sheetViews>
     <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="K74" sqref="K74"/>
@@ -1358,20 +1182,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="74.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="6" max="6" style="2" width="9.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="9" max="9" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="74.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="2" collapsed="1"/>
+    <col min="7" max="8" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" collapsed="1"/>
+    <col min="10" max="11" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>275</v>
+        <v>230</v>
       </c>
       <c r="D3" s="19" t="s">
         <v>7</v>
@@ -1451,7 +1275,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>268</v>
+        <v>223</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>5</v>
@@ -1527,7 +1351,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>267</v>
+        <v>222</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -1558,7 +1382,7 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>278</v>
+        <v>233</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>11</v>
@@ -1640,7 +1464,7 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>274</v>
+        <v>229</v>
       </c>
       <c r="D20" s="7" t="s">
         <v>5</v>
@@ -1716,7 +1540,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>273</v>
+        <v>228</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -1747,7 +1571,7 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>276</v>
+        <v>231</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>14</v>
@@ -1829,7 +1653,7 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>270</v>
+        <v>225</v>
       </c>
       <c r="D33" s="7" t="s">
         <v>5</v>
@@ -1905,7 +1729,7 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>269</v>
+        <v>224</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -1948,7 +1772,7 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>277</v>
+        <v>232</v>
       </c>
       <c r="D42" s="19" t="s">
         <v>17</v>
@@ -2030,7 +1854,7 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>272</v>
+        <v>227</v>
       </c>
       <c r="D46" s="7" t="s">
         <v>5</v>
@@ -2106,7 +1930,7 @@
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>271</v>
+        <v>226</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -2775,12 +2599,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="G96:H96"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="G68:H68"/>
@@ -2791,59 +2615,59 @@
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="J42:K42"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="G55:H55"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="74.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="6" max="6" style="2" width="9.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="9" max="9" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="74.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="2" collapsed="1"/>
+    <col min="7" max="8" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" collapsed="1"/>
+    <col min="10" max="11" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>263</v>
+        <v>218</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>222</v>
+        <v>177</v>
       </c>
       <c r="E3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>223</v>
+        <v>178</v>
       </c>
       <c r="H3" s="19"/>
       <c r="J3" s="19" t="s">
-        <v>224</v>
+        <v>179</v>
       </c>
       <c r="K3" s="19"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D4" s="18" t="s">
         <v>2</v>
@@ -2906,7 +2730,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>256</v>
+        <v>211</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>5</v>
@@ -2917,19 +2741,19 @@
       <c r="G7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="H7" s="8" t="n">
+      <c r="H7" s="8">
         <v>1.5</v>
       </c>
       <c r="J7" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="8" t="n">
+      <c r="K7" s="8">
         <v>1.5</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
@@ -2982,7 +2806,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>255</v>
+        <v>210</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -2993,7 +2817,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -3013,24 +2837,24 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>266</v>
+        <v>221</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>226</v>
+        <v>181</v>
       </c>
       <c r="E16" s="19"/>
       <c r="G16" s="19" t="s">
-        <v>227</v>
+        <v>182</v>
       </c>
       <c r="H16" s="19"/>
       <c r="J16" s="19" t="s">
-        <v>228</v>
+        <v>183</v>
       </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>2</v>
@@ -3095,7 +2919,7 @@
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>262</v>
+        <v>217</v>
       </c>
       <c r="D20" s="18" t="s">
         <v>5</v>
@@ -3118,7 +2942,7 @@
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D21" s="9">
         <v>1</v>
@@ -3171,7 +2995,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>261</v>
+        <v>216</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -3182,7 +3006,7 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -3202,24 +3026,24 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>264</v>
+        <v>219</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>229</v>
+        <v>184</v>
       </c>
       <c r="E29" s="19"/>
       <c r="G29" s="19" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="H29" s="19"/>
       <c r="J29" s="19" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="K29" s="19"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D30" s="18" t="s">
         <v>2</v>
@@ -3284,7 +3108,7 @@
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>258</v>
+        <v>213</v>
       </c>
       <c r="D33" s="18" t="s">
         <v>5</v>
@@ -3307,7 +3131,7 @@
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D34" s="9">
         <v>1</v>
@@ -3360,7 +3184,7 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>257</v>
+        <v>212</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -3371,7 +3195,7 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -3403,24 +3227,24 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>265</v>
+        <v>220</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="E42" s="19"/>
       <c r="G42" s="19" t="s">
-        <v>233</v>
+        <v>188</v>
       </c>
       <c r="H42" s="19"/>
       <c r="J42" s="19" t="s">
-        <v>234</v>
+        <v>189</v>
       </c>
       <c r="K42" s="19"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>2</v>
@@ -3485,7 +3309,7 @@
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>260</v>
+        <v>215</v>
       </c>
       <c r="D46" s="18" t="s">
         <v>5</v>
@@ -3508,7 +3332,7 @@
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D47" s="9">
         <v>1</v>
@@ -3561,7 +3385,7 @@
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>259</v>
+        <v>214</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -3572,7 +3396,7 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -3592,24 +3416,24 @@
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>235</v>
+        <v>190</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
       <c r="E55" s="19"/>
       <c r="G55" s="19" t="s">
-        <v>237</v>
+        <v>192</v>
       </c>
       <c r="H55" s="19"/>
       <c r="J55" s="19" t="s">
-        <v>238</v>
+        <v>193</v>
       </c>
       <c r="K55" s="19"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D56" s="18" t="s">
         <v>2</v>
@@ -3674,7 +3498,7 @@
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>239</v>
+        <v>194</v>
       </c>
       <c r="D59" s="18" t="s">
         <v>5</v>
@@ -3697,7 +3521,7 @@
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D60" s="9">
         <v>1</v>
@@ -3750,7 +3574,7 @@
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -3761,7 +3585,7 @@
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -3775,24 +3599,24 @@
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>241</v>
+        <v>196</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
       <c r="E68" s="19"/>
       <c r="G68" s="19" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="H68" s="19"/>
       <c r="J68" s="19" t="s">
-        <v>244</v>
+        <v>199</v>
       </c>
       <c r="K68" s="19"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D69" s="18" t="s">
         <v>2</v>
@@ -3857,7 +3681,7 @@
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="D72" s="18" t="s">
         <v>5</v>
@@ -3880,7 +3704,7 @@
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D73" s="9">
         <v>1</v>
@@ -3933,7 +3757,7 @@
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>246</v>
+        <v>201</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
@@ -3944,7 +3768,7 @@
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -3982,20 +3806,20 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>254</v>
+        <v>209</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>252</v>
+        <v>207</v>
       </c>
       <c r="E84" s="19"/>
       <c r="G84" s="19" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="H84" s="19"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D85" s="18" t="s">
         <v>2</v>
@@ -4040,7 +3864,7 @@
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>253</v>
+        <v>208</v>
       </c>
       <c r="D88" s="18" t="s">
         <v>5</v>
@@ -4057,7 +3881,7 @@
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D89" s="9">
         <v>1</v>
@@ -4106,20 +3930,20 @@
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>247</v>
+        <v>202</v>
       </c>
       <c r="D96" s="19" t="s">
-        <v>249</v>
+        <v>204</v>
       </c>
       <c r="E96" s="19"/>
       <c r="G96" s="19" t="s">
-        <v>250</v>
+        <v>205</v>
       </c>
       <c r="H96" s="19"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D97" s="18" t="s">
         <v>2</v>
@@ -4164,7 +3988,7 @@
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>248</v>
+        <v>203</v>
       </c>
       <c r="D100" s="18" t="s">
         <v>5</v>
@@ -4181,7 +4005,7 @@
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>225</v>
+        <v>180</v>
       </c>
       <c r="D101" s="9">
         <v>1</v>
@@ -4230,12 +4054,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="G96:H96"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="G68:H68"/>
@@ -4246,58 +4070,58 @@
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="J42:K42"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="G84:H84"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="G96:H96"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="G55:H55"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:K105"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B79" sqref="B79"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E99" sqref="E99:E102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="74.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="6" max="6" style="2" width="9.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="9" max="9" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="74.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.140625" style="2" collapsed="1"/>
+    <col min="7" max="8" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="9.140625" style="2" collapsed="1"/>
+    <col min="10" max="11" width="12.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="12" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="19" t="s">
         <v>132</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>133</v>
       </c>
       <c r="E3" s="19"/>
       <c r="G3" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H3" s="19"/>
       <c r="J3" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K3" s="19"/>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D4" s="17" t="s">
         <v>2</v>
@@ -4343,47 +4167,47 @@
         <v>4</v>
       </c>
       <c r="E6" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G6" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H6" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J6" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K6" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>137</v>
+        <v>167</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H7" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J7" s="17" t="s">
         <v>5</v>
       </c>
       <c r="K7" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D8" s="9">
         <v>1</v>
@@ -4410,19 +4234,19 @@
         <v>6</v>
       </c>
       <c r="E9" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H9" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J9" s="17" t="s">
         <v>6</v>
       </c>
       <c r="K9" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
@@ -4436,7 +4260,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>138</v>
+        <v>168</v>
       </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
@@ -4447,7 +4271,7 @@
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
@@ -4467,24 +4291,24 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>139</v>
+        <v>166</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E16" s="19"/>
       <c r="G16" s="19" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="H16" s="19"/>
       <c r="J16" s="19" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="K16" s="19"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>2</v>
@@ -4532,47 +4356,47 @@
         <v>4</v>
       </c>
       <c r="E19" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G19" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H19" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J19" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K19" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="D20" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E20" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H20" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J20" s="17" t="s">
         <v>5</v>
       </c>
       <c r="K20" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D21" s="9">
         <v>1</v>
@@ -4599,19 +4423,19 @@
         <v>6</v>
       </c>
       <c r="E22" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H22" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J22" s="17" t="s">
         <v>6</v>
       </c>
       <c r="K22" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -4625,7 +4449,7 @@
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>144</v>
+        <v>160</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -4636,7 +4460,7 @@
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -4656,24 +4480,24 @@
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="D29" s="19" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E29" s="19"/>
       <c r="G29" s="19" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="H29" s="19"/>
       <c r="J29" s="19" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="K29" s="19"/>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D30" s="17" t="s">
         <v>2</v>
@@ -4721,47 +4545,47 @@
         <v>4</v>
       </c>
       <c r="E32" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G32" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H32" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J32" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K32" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G33" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H33" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J33" s="17" t="s">
         <v>5</v>
       </c>
       <c r="K33" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D34" s="9">
         <v>1</v>
@@ -4788,19 +4612,19 @@
         <v>6</v>
       </c>
       <c r="E35" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H35" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J35" s="17" t="s">
         <v>6</v>
       </c>
       <c r="K35" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
@@ -4814,7 +4638,7 @@
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -4825,7 +4649,7 @@
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
@@ -4857,24 +4681,24 @@
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E42" s="19"/>
       <c r="G42" s="19" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="H42" s="19"/>
       <c r="J42" s="19" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="K42" s="19"/>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>2</v>
@@ -4922,47 +4746,47 @@
         <v>4</v>
       </c>
       <c r="E45" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G45" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H45" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J45" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K45" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D46" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E46" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G46" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H46" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J46" s="17" t="s">
         <v>5</v>
       </c>
       <c r="K46" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D47" s="9">
         <v>1</v>
@@ -4989,19 +4813,19 @@
         <v>6</v>
       </c>
       <c r="E48" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G48" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H48" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J48" s="17" t="s">
         <v>6</v>
       </c>
       <c r="K48" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
@@ -5015,7 +4839,7 @@
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
@@ -5026,7 +4850,7 @@
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
@@ -5046,24 +4870,24 @@
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>157</v>
+        <v>163</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="E55" s="19"/>
       <c r="G55" s="19" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="H55" s="19"/>
       <c r="J55" s="19" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="K55" s="19"/>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D56" s="17" t="s">
         <v>2</v>
@@ -5111,47 +4935,47 @@
         <v>4</v>
       </c>
       <c r="E58" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G58" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H58" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J58" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K58" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D59" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E59" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G59" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H59" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J59" s="17" t="s">
         <v>5</v>
       </c>
       <c r="K59" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D60" s="9">
         <v>1</v>
@@ -5178,19 +5002,19 @@
         <v>6</v>
       </c>
       <c r="E61" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G61" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H61" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J61" s="17" t="s">
         <v>6</v>
       </c>
       <c r="K61" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
@@ -5204,7 +5028,7 @@
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B63" s="1" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D63" s="3"/>
       <c r="E63" s="3"/>
@@ -5215,7 +5039,7 @@
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
@@ -5229,24 +5053,24 @@
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B68" s="1" t="s">
-        <v>163</v>
+        <v>148</v>
       </c>
       <c r="D68" s="19" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="E68" s="19"/>
       <c r="G68" s="19" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="H68" s="19"/>
       <c r="J68" s="19" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="K68" s="19"/>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B69" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D69" s="17" t="s">
         <v>2</v>
@@ -5294,47 +5118,47 @@
         <v>4</v>
       </c>
       <c r="E71" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G71" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H71" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J71" s="17" t="s">
         <v>4</v>
       </c>
       <c r="K71" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B72" s="1" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="D72" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E72" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G72" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H72" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J72" s="17" t="s">
         <v>5</v>
       </c>
       <c r="K72" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B73" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D73" s="9">
         <v>1</v>
@@ -5361,19 +5185,19 @@
         <v>6</v>
       </c>
       <c r="E74" s="8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G74" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H74" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="J74" s="17" t="s">
         <v>6</v>
       </c>
       <c r="K74" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
@@ -5387,7 +5211,7 @@
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B76" s="1" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
@@ -5398,7 +5222,7 @@
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B77" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
@@ -5436,20 +5260,20 @@
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="1" t="s">
-        <v>213</v>
+        <v>169</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>207</v>
+        <v>174</v>
       </c>
       <c r="E84" s="19"/>
       <c r="G84" s="19" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="H84" s="19"/>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D85" s="17" t="s">
         <v>2</v>
@@ -5483,35 +5307,35 @@
         <v>4</v>
       </c>
       <c r="E87" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G87" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H87" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="1" t="s">
-        <v>212</v>
+        <v>170</v>
       </c>
       <c r="D88" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E88" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G88" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H88" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D89" s="9">
         <v>1</v>
@@ -5531,13 +5355,13 @@
         <v>6</v>
       </c>
       <c r="E90" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G90" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H90" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
@@ -5560,20 +5384,20 @@
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="1" t="s">
-        <v>210</v>
+        <v>171</v>
       </c>
       <c r="D96" s="19" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="E96" s="19"/>
       <c r="G96" s="19" t="s">
-        <v>209</v>
+        <v>176</v>
       </c>
       <c r="H96" s="19"/>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D97" s="17" t="s">
         <v>2</v>
@@ -5607,35 +5431,35 @@
         <v>4</v>
       </c>
       <c r="E99" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G99" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H99" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="1" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="D100" s="17" t="s">
         <v>5</v>
       </c>
       <c r="E100" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G100" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H100" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D101" s="9">
         <v>1</v>
@@ -5655,13 +5479,13 @@
         <v>6</v>
       </c>
       <c r="E102" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G102" s="17" t="s">
         <v>6</v>
       </c>
       <c r="H102" s="8">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
@@ -5684,12 +5508,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="G84:H84"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="G96:H96"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="G55:H55"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="J16:K16"/>
     <mergeCell ref="J55:K55"/>
     <mergeCell ref="D68:E68"/>
     <mergeCell ref="G68:H68"/>
@@ -5700,1489 +5524,35 @@
     <mergeCell ref="D42:E42"/>
     <mergeCell ref="G42:H42"/>
     <mergeCell ref="J42:K42"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
-  </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:L105"/>
-  <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99:E102"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="74.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="2" width="18.7109375" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="6" max="6" style="2" width="9.140625" collapsed="true"/>
-    <col min="7" max="8" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="9" max="9" style="2" width="9.140625" collapsed="true"/>
-    <col min="10" max="11" customWidth="true" style="2" width="12.85546875" collapsed="true"/>
-    <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="E3" s="19"/>
-      <c r="G3" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="H3" s="19"/>
-      <c r="J3" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="K3" s="19"/>
-    </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K4" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="8">
-        <v>0</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="8">
-        <v>2</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="8">
-        <v>2</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K7" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D8" s="9">
-        <v>1</v>
-      </c>
-      <c r="E8" s="8">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="J8" s="9">
-        <v>1</v>
-      </c>
-      <c r="K8" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="D9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="8">
-        <v>0</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H9" s="8">
-        <v>12</v>
-      </c>
-      <c r="J9" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K9" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="4"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="3"/>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="E16" s="19"/>
-      <c r="G16" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="H16" s="19"/>
-      <c r="J16" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E17" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K17" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="3"/>
-      <c r="D18" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="D19" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E19" s="8">
-        <v>0</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H19" s="8">
-        <v>0</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K19" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E20" s="8">
-        <v>2</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="8">
-        <v>2</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K20" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D21" s="9">
-        <v>1</v>
-      </c>
-      <c r="E21" s="8">
-        <v>1</v>
-      </c>
-      <c r="G21" s="9">
-        <v>1</v>
-      </c>
-      <c r="H21" s="8">
-        <v>1</v>
-      </c>
-      <c r="J21" s="9">
-        <v>1</v>
-      </c>
-      <c r="K21" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="3"/>
-      <c r="D22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="8">
-        <v>0</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H22" s="8">
-        <v>12</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K22" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="4"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="4"/>
-      <c r="J23" s="3"/>
-      <c r="K23" s="4"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="J24" s="3"/>
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="J25" s="3"/>
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" s="3"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" s="3"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>176</v>
-      </c>
-      <c r="E29" s="19"/>
-      <c r="G29" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H29" s="19"/>
-      <c r="J29" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="K29" s="19"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D30" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E30" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G30" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K30" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="D31" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G31" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H31" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K31" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="D32" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E32" s="8">
-        <v>0</v>
-      </c>
-      <c r="G32" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H32" s="8">
-        <v>0</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K32" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E33" s="8">
-        <v>2</v>
-      </c>
-      <c r="G33" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="8">
-        <v>2</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K33" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D34" s="9">
-        <v>1</v>
-      </c>
-      <c r="E34" s="8">
-        <v>1</v>
-      </c>
-      <c r="G34" s="9">
-        <v>1</v>
-      </c>
-      <c r="H34" s="8">
-        <v>1</v>
-      </c>
-      <c r="J34" s="9">
-        <v>1</v>
-      </c>
-      <c r="K34" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" s="3"/>
-      <c r="D35" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" s="8">
-        <v>0</v>
-      </c>
-      <c r="G35" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H35" s="8">
-        <v>12</v>
-      </c>
-      <c r="J35" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K35" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="4"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="4"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="4"/>
-    </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="J37" s="3"/>
-      <c r="K37" s="3"/>
-    </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-    </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="4"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="4"/>
-    </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="4"/>
-      <c r="J40" s="3"/>
-      <c r="K40" s="4"/>
-    </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" s="3"/>
-      <c r="G41" s="4"/>
-      <c r="H41" s="4"/>
-      <c r="J41" s="4"/>
-      <c r="K41" s="4"/>
-    </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="E42" s="19"/>
-      <c r="G42" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="H42" s="19"/>
-      <c r="J42" s="19" t="s">
-        <v>181</v>
-      </c>
-      <c r="K42" s="19"/>
-    </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D43" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G43" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H43" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K43" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" s="3"/>
-      <c r="D44" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G44" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K44" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" s="3"/>
-      <c r="D45" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" s="8">
-        <v>0</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H45" s="8">
-        <v>0</v>
-      </c>
-      <c r="J45" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K45" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="D46" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E46" s="8">
-        <v>2</v>
-      </c>
-      <c r="G46" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H46" s="8">
-        <v>2</v>
-      </c>
-      <c r="J46" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K46" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D47" s="9">
-        <v>1</v>
-      </c>
-      <c r="E47" s="8">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
-        <v>1</v>
-      </c>
-      <c r="H47" s="8">
-        <v>1</v>
-      </c>
-      <c r="J47" s="9">
-        <v>1</v>
-      </c>
-      <c r="K47" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" s="3"/>
-      <c r="D48" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="8">
-        <v>0</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H48" s="8">
-        <v>12</v>
-      </c>
-      <c r="J48" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K48" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="4"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="4"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="4"/>
-    </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-    </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-    </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="E55" s="19"/>
-      <c r="G55" s="19" t="s">
-        <v>183</v>
-      </c>
-      <c r="H55" s="19"/>
-      <c r="J55" s="19" t="s">
-        <v>184</v>
-      </c>
-      <c r="K55" s="19"/>
-    </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D56" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E56" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G56" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H56" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J56" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K56" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-      <c r="D57" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E57" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G57" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H57" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J57" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K57" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-      <c r="D58" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E58" s="8">
-        <v>0</v>
-      </c>
-      <c r="G58" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H58" s="8">
-        <v>0</v>
-      </c>
-      <c r="J58" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K58" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E59" s="8">
-        <v>2</v>
-      </c>
-      <c r="G59" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H59" s="8">
-        <v>2</v>
-      </c>
-      <c r="J59" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K59" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D60" s="9">
-        <v>1</v>
-      </c>
-      <c r="E60" s="8">
-        <v>1</v>
-      </c>
-      <c r="G60" s="9">
-        <v>1</v>
-      </c>
-      <c r="H60" s="8">
-        <v>1</v>
-      </c>
-      <c r="J60" s="9">
-        <v>1</v>
-      </c>
-      <c r="K60" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-      <c r="D61" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E61" s="8">
-        <v>0</v>
-      </c>
-      <c r="G61" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H61" s="8">
-        <v>12</v>
-      </c>
-      <c r="J61" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K61" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="4"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="4"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="4"/>
-    </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-    </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-    </row>
-    <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="E68" s="19"/>
-      <c r="G68" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="H68" s="19"/>
-      <c r="J68" s="19" t="s">
-        <v>188</v>
-      </c>
-      <c r="K68" s="19"/>
-    </row>
-    <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B69" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E69" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G69" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H69" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="J69" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="K69" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-      <c r="D70" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E70" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G70" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H70" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="J70" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="K70" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="71" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-      <c r="D71" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E71" s="8">
-        <v>0</v>
-      </c>
-      <c r="G71" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H71" s="8">
-        <v>0</v>
-      </c>
-      <c r="J71" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="K71" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B72" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D72" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E72" s="8">
-        <v>2</v>
-      </c>
-      <c r="G72" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H72" s="8">
-        <v>2</v>
-      </c>
-      <c r="J72" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="K72" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="73" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B73" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D73" s="9">
-        <v>1</v>
-      </c>
-      <c r="E73" s="8">
-        <v>1</v>
-      </c>
-      <c r="G73" s="9">
-        <v>1</v>
-      </c>
-      <c r="H73" s="8">
-        <v>1</v>
-      </c>
-      <c r="J73" s="9">
-        <v>1</v>
-      </c>
-      <c r="K73" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-      <c r="D74" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E74" s="8">
-        <v>0</v>
-      </c>
-      <c r="G74" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H74" s="8">
-        <v>12</v>
-      </c>
-      <c r="J74" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="K74" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="75" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="4"/>
-      <c r="G75" s="3"/>
-      <c r="H75" s="4"/>
-      <c r="J75" s="3"/>
-      <c r="K75" s="4"/>
-    </row>
-    <row r="76" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B76" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="3"/>
-      <c r="J76" s="3"/>
-      <c r="K76" s="3"/>
-    </row>
-    <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="G77" s="3"/>
-      <c r="H77" s="3"/>
-      <c r="J77" s="3"/>
-      <c r="K77" s="3"/>
-    </row>
-    <row r="78" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D78" s="3"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
-    </row>
-    <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="D79" s="3"/>
-      <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="J79" s="4"/>
-      <c r="K79" s="4"/>
-    </row>
-    <row r="80" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-      <c r="D80" s="3"/>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D81" s="3"/>
-    </row>
-    <row r="82" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D82" s="3"/>
-    </row>
-    <row r="83" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D83" s="3"/>
-    </row>
-    <row r="84" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B84" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>219</v>
-      </c>
-      <c r="E84" s="19"/>
-      <c r="G84" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="H84" s="19"/>
-    </row>
-    <row r="85" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B85" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D85" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E85" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G85" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H85" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D86" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E86" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G86" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H86" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D87" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E87" s="8">
-        <v>0</v>
-      </c>
-      <c r="G87" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H87" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B88" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="D88" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E88" s="8">
-        <v>2</v>
-      </c>
-      <c r="G88" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H88" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B89" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D89" s="9">
-        <v>1</v>
-      </c>
-      <c r="E89" s="8">
-        <v>1</v>
-      </c>
-      <c r="G89" s="9">
-        <v>1</v>
-      </c>
-      <c r="H89" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D90" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E90" s="8">
-        <v>12</v>
-      </c>
-      <c r="G90" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H90" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="91" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D91" s="3"/>
-      <c r="E91" s="4"/>
-      <c r="G91" s="3"/>
-      <c r="H91" s="4"/>
-    </row>
-    <row r="92" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-      <c r="G92" s="3"/>
-      <c r="H92" s="3"/>
-    </row>
-    <row r="93" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
-      <c r="G93" s="3"/>
-      <c r="H93" s="3"/>
-    </row>
-    <row r="96" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B96" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="D96" s="19" t="s">
-        <v>218</v>
-      </c>
-      <c r="E96" s="19"/>
-      <c r="G96" s="19" t="s">
-        <v>221</v>
-      </c>
-      <c r="H96" s="19"/>
-    </row>
-    <row r="97" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B97" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D97" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="E97" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="G97" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H97" s="17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D98" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="E98" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="G98" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="H98" s="17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="E99" s="8">
-        <v>0</v>
-      </c>
-      <c r="G99" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="H99" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B100" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D100" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="E100" s="8">
-        <v>2</v>
-      </c>
-      <c r="G100" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="H100" s="8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="101" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B101" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D101" s="9">
-        <v>1</v>
-      </c>
-      <c r="E101" s="8">
-        <v>1</v>
-      </c>
-      <c r="G101" s="9">
-        <v>1</v>
-      </c>
-      <c r="H101" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D102" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E102" s="8">
-        <v>12</v>
-      </c>
-      <c r="G102" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="H102" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="103" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D103" s="3"/>
-      <c r="E103" s="4"/>
-      <c r="G103" s="3"/>
-      <c r="H103" s="4"/>
-    </row>
-    <row r="104" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D104" s="3"/>
-      <c r="E104" s="3"/>
-      <c r="G104" s="3"/>
-      <c r="H104" s="3"/>
-    </row>
-    <row r="105" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="D105" s="3"/>
-      <c r="E105" s="3"/>
-      <c r="G105" s="3"/>
-      <c r="H105" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="22">
     <mergeCell ref="D84:E84"/>
     <mergeCell ref="G84:H84"/>
     <mergeCell ref="D96:E96"/>
     <mergeCell ref="G96:H96"/>
     <mergeCell ref="D55:E55"/>
     <mergeCell ref="G55:H55"/>
-    <mergeCell ref="J55:K55"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="G68:H68"/>
-    <mergeCell ref="J68:K68"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="J16:K16"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:P103"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:O103"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" workbookViewId="0" zoomScale="115" zoomScaleNormal="115">
+    <sheetView topLeftCell="A79" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C95" sqref="C95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="103.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="24.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="2" width="24.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="82.85546875" collapsed="true"/>
-    <col min="8" max="8" style="2" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="57.0" collapsed="true"/>
-    <col min="12" max="12" style="2" width="9.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="44.7109375" collapsed="true"/>
+    <col min="2" max="2" width="103.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="24" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="82.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.140625" style="2" collapsed="1"/>
+    <col min="9" max="9" width="57" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.140625" style="2" collapsed="1"/>
+    <col min="14" max="14" width="44.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
@@ -9565,6 +7935,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="D97:F97"/>
+    <mergeCell ref="D85:F85"/>
+    <mergeCell ref="D69:F69"/>
+    <mergeCell ref="D56:F56"/>
+    <mergeCell ref="D43:F43"/>
     <mergeCell ref="H85:J85"/>
     <mergeCell ref="H97:J97"/>
     <mergeCell ref="L4:N4"/>
@@ -9578,22 +7956,14 @@
     <mergeCell ref="H43:J43"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="D97:F97"/>
-    <mergeCell ref="D85:F85"/>
-    <mergeCell ref="D69:F69"/>
-    <mergeCell ref="D56:F56"/>
-    <mergeCell ref="D43:F43"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:O103"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:N103"/>
   <sheetViews>
     <sheetView topLeftCell="C61" workbookViewId="0">
       <selection activeCell="F100" sqref="F100:F103"/>
@@ -9601,15 +7971,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="9.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="103.7109375" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="2" width="24.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="2" width="82.85546875" collapsed="true"/>
-    <col min="6" max="8" style="2" width="9.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="2" width="57.0" collapsed="true"/>
-    <col min="10" max="13" style="2" width="9.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="2" width="44.7109375" collapsed="true"/>
-    <col min="15" max="16384" style="2" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.140625" style="2" collapsed="1"/>
+    <col min="2" max="2" width="103.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="24" style="2" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="82.85546875" style="2" customWidth="1" collapsed="1"/>
+    <col min="6" max="8" width="9.140625" style="2" collapsed="1"/>
+    <col min="9" max="9" width="57" style="2" customWidth="1" collapsed="1"/>
+    <col min="10" max="13" width="9.140625" style="2" collapsed="1"/>
+    <col min="14" max="14" width="44.7109375" style="2" customWidth="1" collapsed="1"/>
+    <col min="15" max="16384" width="9.140625" style="2" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:14" x14ac:dyDescent="0.25">
@@ -11418,6 +9788,18 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="H4:J4"/>
+    <mergeCell ref="L4:N4"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="D30:F30"/>
+    <mergeCell ref="H30:J30"/>
+    <mergeCell ref="L30:N30"/>
+    <mergeCell ref="D43:F43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="L43:N43"/>
     <mergeCell ref="D97:F97"/>
     <mergeCell ref="H97:J97"/>
     <mergeCell ref="D56:F56"/>
@@ -11427,19 +9809,7 @@
     <mergeCell ref="H69:J69"/>
     <mergeCell ref="D85:F85"/>
     <mergeCell ref="H85:J85"/>
-    <mergeCell ref="D30:F30"/>
-    <mergeCell ref="H30:J30"/>
-    <mergeCell ref="L30:N30"/>
-    <mergeCell ref="D43:F43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="L43:N43"/>
-    <mergeCell ref="D4:F4"/>
-    <mergeCell ref="H4:J4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="L17:N17"/>
   </mergeCells>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>